<commit_message>
database design for time & add view lists
</commit_message>
<xml_diff>
--- a/database_design.xlsx
+++ b/database_design.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
   <si>
     <t>Users Table</t>
   </si>
@@ -80,10 +80,37 @@
     <t>Role Table</t>
   </si>
   <si>
-    <t>created_at</t>
-  </si>
-  <si>
-    <t>updated_at</t>
+    <t>created_by</t>
+  </si>
+  <si>
+    <t>updated_by</t>
+  </si>
+  <si>
+    <t>Appointment</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>Appointment Time</t>
+  </si>
+  <si>
+    <t>time_id</t>
+  </si>
+  <si>
+    <t>appointment_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Time</t>
+  </si>
+  <si>
+    <t>Doctor Appointment Management System</t>
   </si>
 </sst>
 </file>
@@ -106,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +164,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -185,37 +218,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,196 +588,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L22"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="3" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="3" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="5"/>
+    <col min="7" max="7" width="11.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.42578125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="5"/>
+    <col min="11" max="11" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.5703125" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="F3" s="10" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="F3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="D4" s="11"/>
+      <c r="F4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="H4" s="11"/>
+      <c r="J4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="F5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="9" t="s">
+      <c r="F5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="J5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="H6" s="14"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="J7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="F9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="10"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+      <c r="F10" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="J10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+      <c r="F11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="F12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="J12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" s="16"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+      <c r="F13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="16"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="F14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="16"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="9" t="s">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="3"/>
@@ -712,22 +944,49 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="F3:H3"/>
   </mergeCells>
+  <conditionalFormatting sqref="A1:N1">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3FD0DD17-5EF0-4979-9D0F-4497DC96FF58}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3FD0DD17-5EF0-4979-9D0F-4497DC96FF58}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>A1:N1</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>